<commit_message>
Added comments to all metadata tests  and methods to better describe its purpose. All  SEO metadata testcases are descirpbed in https://github.com/NCIOCPL/cgov-digital-platform-qa/issues/90. This push also includes updated chromedriver.
</commit_message>
<xml_diff>
--- a/test-data/meta_data.xlsx
+++ b/test-data/meta_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC794D69-C11B-374A-A31F-9BEC03245095}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A381DB7-B910-244D-BE05-55403A60BB6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="3920" windowWidth="29360" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="4260" windowWidth="29360" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_meta_Issued_date" sheetId="4" r:id="rId1"/>
@@ -338,12 +338,6 @@
     <t>Blinatumomab</t>
   </si>
   <si>
-    <t>Prurito</t>
-  </si>
-  <si>
-    <t>Pruritus</t>
-  </si>
-  <si>
     <t>Key Initiatives</t>
   </si>
   <si>
@@ -428,12 +422,6 @@
     <t>24/04/2019 - 08:00</t>
   </si>
   <si>
-    <t>07/29/2019 - 08:00</t>
-  </si>
-  <si>
-    <t>29/07/2019 - 08:00</t>
-  </si>
-  <si>
     <t>03/11/2019 - 08:00</t>
   </si>
   <si>
@@ -441,13 +429,25 @@
   </si>
   <si>
     <t>12/22/2014 - 07:00</t>
+  </si>
+  <si>
+    <t>08/10/2019 - 08:00</t>
+  </si>
+  <si>
+    <t>Pruritus (PDQ®)–Patient Version</t>
+  </si>
+  <si>
+    <t>Prurito (PDQ®)–Versión para profesionales de salud</t>
+  </si>
+  <si>
+    <t>10/08/2019 - 08:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +462,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1A1AA6"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -484,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -497,6 +509,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796F7A8F-3D9B-B242-8B0D-5F47A2331775}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -796,7 +809,7 @@
     <col min="4" max="16384" width="22.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -804,10 +817,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -815,10 +828,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -826,10 +839,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
@@ -837,10 +850,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
@@ -848,10 +861,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -859,10 +872,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
@@ -870,10 +883,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -881,10 +894,10 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -892,10 +905,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -903,10 +916,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
@@ -914,10 +927,10 @@
         <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
@@ -925,10 +938,11 @@
         <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
@@ -936,10 +950,10 @@
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
@@ -947,10 +961,10 @@
         <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
@@ -958,10 +972,10 @@
         <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -969,7 +983,7 @@
         <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -980,10 +994,11 @@
         <v>62</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -993,14 +1008,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="70.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
@@ -1049,7 +1064,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>70</v>
@@ -1081,7 +1096,7 @@
         <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>76</v>
@@ -1113,7 +1128,7 @@
         <v>98</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>99</v>
@@ -1145,7 +1160,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>79</v>
@@ -1177,7 +1192,7 @@
         <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>80</v>
@@ -1209,7 +1224,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>80</v>
@@ -1241,7 +1256,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>81</v>
@@ -1305,7 +1320,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>83</v>
@@ -1337,7 +1352,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>83</v>
@@ -1369,7 +1384,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>84</v>
@@ -1401,7 +1416,7 @@
         <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>85</v>
@@ -1433,7 +1448,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>86</v>
@@ -1465,7 +1480,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>87</v>
@@ -1497,7 +1512,7 @@
         <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>88</v>
@@ -1529,7 +1544,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>89</v>
@@ -1561,7 +1576,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>90</v>
@@ -1593,7 +1608,7 @@
         <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>74</v>
@@ -1625,7 +1640,7 @@
         <v>94</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>95</v>
@@ -1657,7 +1672,7 @@
         <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>91</v>
@@ -1689,7 +1704,7 @@
         <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>92</v>

</xml_diff>